<commit_message>
Correction numéro de SIRET
</commit_message>
<xml_diff>
--- a/exemple-valide.xlsx
+++ b/exemple-valide.xlsx
@@ -5,9 +5,7 @@
   <sheets>
     <sheet state="visible" name="Worksheet" sheetId="1" r:id="rId4"/>
   </sheets>
-  <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Worksheet!$A$1:$AD$2</definedName>
-  </definedNames>
+  <definedNames/>
   <calcPr/>
 </workbook>
 </file>
@@ -126,7 +124,7 @@
     <t>true</t>
   </si>
   <si>
-    <t>80295478500028</t>
+    <t>21920044100018</t>
   </si>
   <si>
     <t>ouvrage</t>
@@ -387,17 +385,17 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="30" width="9.14"/>
+    <col customWidth="1" min="1" max="30" width="8.71"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -442,7 +440,7 @@
       <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="1" t="s">
@@ -482,7 +480,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>30</v>
       </c>
@@ -575,7 +573,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$AD$2"/>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Change Non Applicable Value to N/A instead of NA
</commit_message>
<xml_diff>
--- a/exemple-valide.xlsx
+++ b/exemple-valide.xlsx
@@ -1,17 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geoff\Downloads\statio\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34B1C9E-ACA8-4CA8-B86C-47CC14693084}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Worksheet" sheetId="1" r:id="rId4"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Worksheet!$A$1:$AD$2</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
   <si>
     <t>id</t>
   </si>
@@ -124,65 +146,91 @@
     <t>true</t>
   </si>
   <si>
+    <t>ouvrage</t>
+  </si>
+  <si>
+    <t>Gratuité pour le marché le samedi matin</t>
+  </si>
+  <si>
+    <t>75114-P-002</t>
+  </si>
+  <si>
+    <t>290</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
     <t>21920044100018</t>
-  </si>
-  <si>
-    <t>ouvrage</t>
-  </si>
-  <si>
-    <t>Gratuité pour le marché le samedi matin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
-    <font/>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -372,30 +420,34 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AD3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="30" width="8.71"/>
+    <col min="1" max="16" width="9.109375" customWidth="1"/>
+    <col min="17" max="17" width="9.109375" style="4" customWidth="1"/>
+    <col min="18" max="30" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -437,10 +489,10 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="1" t="s">
@@ -480,7 +532,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="2" spans="1:30">
       <c r="A2" s="1" t="s">
         <v>30</v>
       </c>
@@ -503,43 +555,43 @@
         <v>36</v>
       </c>
       <c r="H2" s="1">
-        <v>325.0</v>
+        <v>325</v>
       </c>
       <c r="I2" s="1">
-        <v>250.0</v>
+        <v>250</v>
       </c>
       <c r="J2" s="1">
-        <v>250.0</v>
+        <v>250</v>
       </c>
       <c r="K2" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="L2" s="1">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="M2" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="N2" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="O2" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="P2" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>37</v>
+        <v>5</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="S2" s="1">
         <v>1.452323</v>
       </c>
       <c r="T2" s="1">
-        <v>46.59698</v>
+        <v>46.596980000000002</v>
       </c>
       <c r="U2" s="1" t="s">
         <v>6</v>
@@ -557,25 +609,116 @@
         <v>13.5</v>
       </c>
       <c r="Z2" s="1">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="AA2" s="1">
         <v>60.99</v>
       </c>
       <c r="AB2" s="1">
-        <v>79.99</v>
+        <v>79.989999999999995</v>
       </c>
       <c r="AC2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AD2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:30">
+      <c r="A3" s="1" t="s">
         <v>39</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="1">
+        <v>325</v>
+      </c>
+      <c r="I3" s="1">
+        <v>250</v>
+      </c>
+      <c r="J3" s="1">
+        <v>250</v>
+      </c>
+      <c r="K3" s="1">
+        <v>10</v>
+      </c>
+      <c r="L3" s="1">
+        <v>25</v>
+      </c>
+      <c r="M3" s="1">
+        <v>5</v>
+      </c>
+      <c r="N3" s="1">
+        <v>5</v>
+      </c>
+      <c r="O3" s="1">
+        <v>5</v>
+      </c>
+      <c r="P3" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="S3" s="1">
+        <v>1.452323</v>
+      </c>
+      <c r="T3" s="1">
+        <v>46.596980000000002</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="V3" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="W3" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="X3" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>13.5</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>40</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>60.99</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>79.989999999999995</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <autoFilter ref="A1:AD2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Version 0.1.2 : correction d'un numéro de SIRET (#5)
* Mise à jour dépendances

* Correction numéro de SIRET

* Passage en version 0.1.2
</commit_message>
<xml_diff>
--- a/exemple-valide.xlsx
+++ b/exemple-valide.xlsx
@@ -5,9 +5,7 @@
   <sheets>
     <sheet state="visible" name="Worksheet" sheetId="1" r:id="rId4"/>
   </sheets>
-  <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Worksheet!$A$1:$AD$2</definedName>
-  </definedNames>
+  <definedNames/>
   <calcPr/>
 </workbook>
 </file>
@@ -126,7 +124,7 @@
     <t>true</t>
   </si>
   <si>
-    <t>80295478500028</t>
+    <t>21920044100018</t>
   </si>
   <si>
     <t>ouvrage</t>
@@ -387,17 +385,17 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="30" width="9.14"/>
+    <col customWidth="1" min="1" max="30" width="8.71"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -442,7 +440,7 @@
       <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="1" t="s">
@@ -482,7 +480,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>30</v>
       </c>
@@ -575,7 +573,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$AD$2"/>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Update hauteur_max in Schema (#7)
* Modify schema for hauteur-max field

* Correct regex + update version in schema

* Update valide csv

* Change Non Applicable Value to N/A instead of NA

* Change minor version 0.1.2 to 0.1.3
</commit_message>
<xml_diff>
--- a/exemple-valide.xlsx
+++ b/exemple-valide.xlsx
@@ -1,17 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geoff\Downloads\statio\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34B1C9E-ACA8-4CA8-B86C-47CC14693084}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Worksheet" sheetId="1" r:id="rId4"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Worksheet!$A$1:$AD$2</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
   <si>
     <t>id</t>
   </si>
@@ -124,65 +146,91 @@
     <t>true</t>
   </si>
   <si>
+    <t>ouvrage</t>
+  </si>
+  <si>
+    <t>Gratuité pour le marché le samedi matin</t>
+  </si>
+  <si>
+    <t>75114-P-002</t>
+  </si>
+  <si>
+    <t>290</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
     <t>21920044100018</t>
-  </si>
-  <si>
-    <t>ouvrage</t>
-  </si>
-  <si>
-    <t>Gratuité pour le marché le samedi matin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
-    <font/>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -372,30 +420,34 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AD3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="30" width="8.71"/>
+    <col min="1" max="16" width="9.109375" customWidth="1"/>
+    <col min="17" max="17" width="9.109375" style="4" customWidth="1"/>
+    <col min="18" max="30" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -437,10 +489,10 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="1" t="s">
@@ -480,7 +532,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="2" spans="1:30">
       <c r="A2" s="1" t="s">
         <v>30</v>
       </c>
@@ -503,43 +555,43 @@
         <v>36</v>
       </c>
       <c r="H2" s="1">
-        <v>325.0</v>
+        <v>325</v>
       </c>
       <c r="I2" s="1">
-        <v>250.0</v>
+        <v>250</v>
       </c>
       <c r="J2" s="1">
-        <v>250.0</v>
+        <v>250</v>
       </c>
       <c r="K2" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="L2" s="1">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="M2" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="N2" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="O2" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="P2" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>37</v>
+        <v>5</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="S2" s="1">
         <v>1.452323</v>
       </c>
       <c r="T2" s="1">
-        <v>46.59698</v>
+        <v>46.596980000000002</v>
       </c>
       <c r="U2" s="1" t="s">
         <v>6</v>
@@ -557,25 +609,116 @@
         <v>13.5</v>
       </c>
       <c r="Z2" s="1">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="AA2" s="1">
         <v>60.99</v>
       </c>
       <c r="AB2" s="1">
-        <v>79.99</v>
+        <v>79.989999999999995</v>
       </c>
       <c r="AC2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AD2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:30">
+      <c r="A3" s="1" t="s">
         <v>39</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="1">
+        <v>325</v>
+      </c>
+      <c r="I3" s="1">
+        <v>250</v>
+      </c>
+      <c r="J3" s="1">
+        <v>250</v>
+      </c>
+      <c r="K3" s="1">
+        <v>10</v>
+      </c>
+      <c r="L3" s="1">
+        <v>25</v>
+      </c>
+      <c r="M3" s="1">
+        <v>5</v>
+      </c>
+      <c r="N3" s="1">
+        <v>5</v>
+      </c>
+      <c r="O3" s="1">
+        <v>5</v>
+      </c>
+      <c r="P3" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="S3" s="1">
+        <v>1.452323</v>
+      </c>
+      <c r="T3" s="1">
+        <v>46.596980000000002</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="V3" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="W3" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="X3" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>13.5</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>40</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>60.99</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>79.989999999999995</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <autoFilter ref="A1:AD2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>